<commit_message>
update at 12:20 14/12
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2352fcdd8a7d209/Documents/טכניון/הסמכה/שנה ב/מסדי נתונים/HW/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2352fcdd8a7d209/Documents/טכניון/הסמכה/שנה ב/מסדי נתונים/HW/Project/databaseproject2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{0EBBAC81-3CC1-4DD4-A04B-DFAD73999514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4EC42BF9-3675-4CDB-9D80-0472E43E8CB6}"/>
+  <xr:revisionPtr revIDLastSave="63" documentId="8_{0EBBAC81-3CC1-4DD4-A04B-DFAD73999514}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C2543E3-EF20-40EA-A98F-210A799D3037}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D333B662-8AFF-4248-A8A3-32DB9A3A5087}"/>
+    <workbookView xWindow="1065" yWindow="1110" windowWidth="14310" windowHeight="7410" xr2:uid="{D333B662-8AFF-4248-A8A3-32DB9A3A5087}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$1:$E$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -333,7 +332,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +344,12 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -417,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -426,6 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -742,8 +748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C06A1B9-EF88-4A3B-B0E4-7FA687E96C35}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,73 +999,73 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="1"/>
+      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="1"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -1075,112 +1081,112 @@
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="1"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="1"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E29" s="1"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">

</xml_diff>